<commit_message>
changed data file and added formatting
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/CAPEX OPEX Per Technology.xlsx
+++ b/mppsteel/data/import_data/CAPEX OPEX Per Technology.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{D1A03796-A78E-4FC3-9712-F10AC328032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCD1C5DA-3B42-475E-9FD7-CF25EB1454D0}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{D1A03796-A78E-4FC3-9712-F10AC328032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78092770-0552-475D-A277-A8330F8657D0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5B88B727-8630-4BCE-A967-4A2C273300FC}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" activeTab="1" xr2:uid="{5B88B727-8630-4BCE-A967-4A2C273300FC}"/>
   </bookViews>
   <sheets>
     <sheet name="GF capex" sheetId="1" r:id="rId1"/>
     <sheet name="Renewal capex" sheetId="2" r:id="rId2"/>
     <sheet name="Other Opex" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+  <si>
+    <t>Technology</t>
+  </si>
   <si>
     <t>Avg BF-BOF</t>
   </si>
@@ -65,10 +68,19 @@
     <t>BAT BF-BOF_bio PCI</t>
   </si>
   <si>
+    <t>BAT BF-BOF+CCUS</t>
+  </si>
+  <si>
+    <t>Smelting Reduction+CCUS</t>
+  </si>
+  <si>
     <t>Charcoal mini furnace</t>
   </si>
   <si>
     <t>Electrolyzer-EAF</t>
+  </si>
+  <si>
+    <t>DRI-EAF+CCUS</t>
   </si>
   <si>
     <t>DRI-EAF_100% green H2</t>
@@ -80,7 +92,10 @@
     <t>EAF</t>
   </si>
   <si>
-    <t>BAT BF-BOF+CCUS</t>
+    <t>BAT BF-BOF+CCU</t>
+  </si>
+  <si>
+    <t>DRI-Melt-BOF+CCUS</t>
   </si>
   <si>
     <t>DRI-Melt-BOF_100% zero-C H2</t>
@@ -89,40 +104,7 @@
     <t>Electrowinning-EAF</t>
   </si>
   <si>
-    <t>Initial</t>
-  </si>
-  <si>
-    <t>Trans</t>
-  </si>
-  <si>
-    <t>End-state</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Available from</t>
-  </si>
-  <si>
-    <t>Available until</t>
-  </si>
-  <si>
-    <t>Technology type</t>
-  </si>
-  <si>
-    <t>Smelting Reduction+CCUS</t>
-  </si>
-  <si>
     <t>BAT BF-BOF+BECCUS</t>
-  </si>
-  <si>
-    <t>DRI-Melt-BOF+CCUS</t>
-  </si>
-  <si>
-    <t>BAT BF-BOF+CCU</t>
-  </si>
-  <si>
-    <t>DRI-EAF+CCUS</t>
   </si>
 </sst>
 </file>
@@ -480,14 +462,14 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -583,9 +565,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>871.85064220183472</v>
@@ -681,9 +663,9 @@
         <v>871.85064220183472</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1066.8506422018347</v>
@@ -779,9 +761,9 @@
         <v>1066.8506422018347</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>698.34183486238533</v>
@@ -877,9 +859,9 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>599.46638642822097</v>
@@ -975,9 +957,9 @@
         <v>357.7963864282209</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>603.34183486238533</v>
@@ -1073,9 +1055,9 @@
         <v>603.34183486238533</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>698.34183486238533</v>
@@ -1171,9 +1153,9 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>698.34183486238533</v>
@@ -1269,9 +1251,9 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>1066.8506422018347</v>
@@ -1367,9 +1349,9 @@
         <v>1066.8506422018347</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>1066.8506422018347</v>
@@ -1465,9 +1447,9 @@
         <v>1066.8506422018347</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>1230.0944923998388</v>
@@ -1563,9 +1545,9 @@
         <v>1188.37661957146</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>646.13638642822093</v>
@@ -1661,9 +1643,9 @@
         <v>404.46638642822091</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>206.07533632286996</v>
@@ -1759,9 +1741,9 @@
         <v>206.07533632286996</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>709.87</v>
@@ -1857,9 +1839,9 @@
         <v>662.34</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>843.10492686238535</v>
@@ -1955,9 +1937,9 @@
         <v>752.22587466238531</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>698.34183486238533</v>
@@ -2053,9 +2035,9 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2151,9 +2133,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>210</v>
@@ -2249,9 +2231,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>1298.549525531806</v>
@@ -2347,9 +2329,9 @@
         <v>1239.3375886808133</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>666.58592520512366</v>
@@ -2445,9 +2427,9 @@
         <v>650.42354656197949</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>603.34183486238533</v>
@@ -2543,9 +2525,9 @@
         <v>603.34183486238533</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>744.6</v>
@@ -2641,9 +2623,9 @@
         <v>652.79999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>1279.3610678419107</v>
@@ -2746,139 +2728,127 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F3D0DF-0035-4729-81FE-EF9D246469F5}">
-  <dimension ref="A1:AI23"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
       </c>
       <c r="E1">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="G1">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="H1">
-        <v>2023</v>
+        <v>2026</v>
       </c>
       <c r="I1">
-        <v>2024</v>
+        <v>2027</v>
       </c>
       <c r="J1">
-        <v>2025</v>
+        <v>2028</v>
       </c>
       <c r="K1">
-        <v>2026</v>
+        <v>2029</v>
       </c>
       <c r="L1">
-        <v>2027</v>
+        <v>2030</v>
       </c>
       <c r="M1">
-        <v>2028</v>
+        <v>2031</v>
       </c>
       <c r="N1">
-        <v>2029</v>
+        <v>2032</v>
       </c>
       <c r="O1">
-        <v>2030</v>
+        <v>2033</v>
       </c>
       <c r="P1">
-        <v>2031</v>
+        <v>2034</v>
       </c>
       <c r="Q1">
-        <v>2032</v>
+        <v>2035</v>
       </c>
       <c r="R1">
-        <v>2033</v>
+        <v>2036</v>
       </c>
       <c r="S1">
-        <v>2034</v>
+        <v>2037</v>
       </c>
       <c r="T1">
-        <v>2035</v>
+        <v>2038</v>
       </c>
       <c r="U1">
-        <v>2036</v>
+        <v>2039</v>
       </c>
       <c r="V1">
-        <v>2037</v>
+        <v>2040</v>
       </c>
       <c r="W1">
-        <v>2038</v>
+        <v>2041</v>
       </c>
       <c r="X1">
-        <v>2039</v>
+        <v>2042</v>
       </c>
       <c r="Y1">
-        <v>2040</v>
+        <v>2043</v>
       </c>
       <c r="Z1">
-        <v>2041</v>
+        <v>2044</v>
       </c>
       <c r="AA1">
-        <v>2042</v>
+        <v>2045</v>
       </c>
       <c r="AB1">
-        <v>2043</v>
+        <v>2046</v>
       </c>
       <c r="AC1">
-        <v>2044</v>
+        <v>2047</v>
       </c>
       <c r="AD1">
-        <v>2045</v>
+        <v>2048</v>
       </c>
       <c r="AE1">
-        <v>2046</v>
+        <v>2049</v>
       </c>
       <c r="AF1">
-        <v>2047</v>
-      </c>
-      <c r="AG1">
-        <v>2048</v>
-      </c>
-      <c r="AH1">
-        <v>2049</v>
-      </c>
-      <c r="AI1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2020</v>
+        <v>187.5</v>
       </c>
       <c r="C2">
-        <v>2030</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
+        <v>187.5</v>
+      </c>
+      <c r="D2">
+        <v>187.5</v>
       </c>
       <c r="E2">
         <v>187.5</v>
@@ -2964,28 +2934,19 @@
       <c r="AF2">
         <v>187.5</v>
       </c>
-      <c r="AG2">
-        <v>187.5</v>
-      </c>
-      <c r="AH2">
-        <v>187.5</v>
-      </c>
-      <c r="AI2">
-        <v>187.5</v>
-      </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>2020</v>
+        <v>285</v>
       </c>
       <c r="C3">
-        <v>2030</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
+        <v>285</v>
+      </c>
+      <c r="D3">
+        <v>285</v>
       </c>
       <c r="E3">
         <v>285</v>
@@ -3071,28 +3032,19 @@
       <c r="AF3">
         <v>285</v>
       </c>
-      <c r="AG3">
-        <v>285</v>
-      </c>
-      <c r="AH3">
-        <v>285</v>
-      </c>
-      <c r="AI3">
-        <v>285</v>
-      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>2020</v>
+        <v>186.55603236551863</v>
       </c>
       <c r="C4">
-        <v>2030</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
+        <v>186.55603236551863</v>
+      </c>
+      <c r="D4">
+        <v>186.55603236551863</v>
       </c>
       <c r="E4">
         <v>186.55603236551863</v>
@@ -3178,135 +3130,117 @@
       <c r="AF4">
         <v>186.55603236551863</v>
       </c>
-      <c r="AG4">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AH4">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AI4">
-        <v>186.55603236551863</v>
-      </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>2028</v>
+        <v>160.14230424929596</v>
       </c>
       <c r="C5">
-        <v>2030</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
+        <v>154.00154406385184</v>
+      </c>
+      <c r="D5">
+        <v>148.09625529760518</v>
       </c>
       <c r="E5">
-        <v>160.14230424929596</v>
+        <v>142.41740864675901</v>
       </c>
       <c r="F5">
-        <v>154.00154406385184</v>
+        <v>136.95632104200769</v>
       </c>
       <c r="G5">
-        <v>148.09625529760518</v>
+        <v>131.70464237195156</v>
       </c>
       <c r="H5">
-        <v>142.41740864675901</v>
+        <v>126.6543427156108</v>
       </c>
       <c r="I5">
-        <v>136.95632104200769</v>
+        <v>121.79770006451669</v>
       </c>
       <c r="J5">
-        <v>131.70464237195156</v>
+        <v>117.12728851560745</v>
       </c>
       <c r="K5">
-        <v>126.6543427156108</v>
+        <v>112.63596691687485</v>
       </c>
       <c r="L5">
-        <v>121.79770006451669</v>
+        <v>108.31686794840103</v>
       </c>
       <c r="M5">
-        <v>117.12728851560745</v>
+        <v>107.64160092698607</v>
       </c>
       <c r="N5">
-        <v>112.63596691687485</v>
+        <v>106.97054364278793</v>
       </c>
       <c r="O5">
-        <v>108.31686794840103</v>
+        <v>106.30366985154045</v>
       </c>
       <c r="P5">
-        <v>107.64160092698607</v>
+        <v>105.64095347258899</v>
       </c>
       <c r="Q5">
-        <v>106.97054364278793</v>
+        <v>104.98236858787045</v>
       </c>
       <c r="R5">
-        <v>106.30366985154045</v>
+        <v>104.32788944089965</v>
       </c>
       <c r="S5">
-        <v>105.64095347258899</v>
+        <v>103.67749043576202</v>
       </c>
       <c r="T5">
-        <v>104.98236858787045</v>
+        <v>103.03114613611255</v>
       </c>
       <c r="U5">
-        <v>104.32788944089965</v>
+        <v>102.38883126418102</v>
       </c>
       <c r="V5">
-        <v>103.67749043576202</v>
+        <v>101.75052069978345</v>
       </c>
       <c r="W5">
-        <v>103.03114613611255</v>
+        <v>101.11618947933961</v>
       </c>
       <c r="X5">
-        <v>102.38883126418102</v>
+        <v>100.48581279489679</v>
       </c>
       <c r="Y5">
-        <v>101.75052069978345</v>
+        <v>99.859365993159557</v>
       </c>
       <c r="Z5">
-        <v>101.11618947933961</v>
+        <v>99.236824574525585</v>
       </c>
       <c r="AA5">
-        <v>100.48581279489679</v>
+        <v>98.618164192127523</v>
       </c>
       <c r="AB5">
-        <v>99.859365993159557</v>
+        <v>98.003360650880822</v>
       </c>
       <c r="AC5">
-        <v>99.236824574525585</v>
+        <v>97.39238990653746</v>
       </c>
       <c r="AD5">
-        <v>98.618164192127523</v>
+        <v>96.785228064745652</v>
       </c>
       <c r="AE5">
-        <v>98.003360650880822</v>
+        <v>96.181851380115319</v>
       </c>
       <c r="AF5">
-        <v>97.39238990653746</v>
-      </c>
-      <c r="AG5">
-        <v>96.785228064745652</v>
-      </c>
-      <c r="AH5">
-        <v>96.181851380115319</v>
-      </c>
-      <c r="AI5">
         <v>95.582236255289374</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>2026</v>
+        <v>161.17759706353402</v>
       </c>
       <c r="C6">
-        <v>2030</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
+        <v>161.17759706353402</v>
+      </c>
+      <c r="D6">
+        <v>161.17759706353402</v>
       </c>
       <c r="E6">
         <v>161.17759706353402</v>
@@ -3392,28 +3326,19 @@
       <c r="AF6">
         <v>161.17759706353402</v>
       </c>
-      <c r="AG6">
-        <v>161.17759706353402</v>
-      </c>
-      <c r="AH6">
-        <v>161.17759706353402</v>
-      </c>
-      <c r="AI6">
-        <v>161.17759706353402</v>
-      </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>2020</v>
+        <v>186.55603236551863</v>
       </c>
       <c r="C7">
-        <v>2030</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
+        <v>186.55603236551863</v>
+      </c>
+      <c r="D7">
+        <v>186.55603236551863</v>
       </c>
       <c r="E7">
         <v>186.55603236551863</v>
@@ -3499,28 +3424,19 @@
       <c r="AF7">
         <v>186.55603236551863</v>
       </c>
-      <c r="AG7">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AH7">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AI7">
-        <v>186.55603236551863</v>
-      </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>2025</v>
+        <v>186.55603236551863</v>
       </c>
       <c r="C8">
-        <v>2030</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
+        <v>186.55603236551863</v>
+      </c>
+      <c r="D8">
+        <v>186.55603236551863</v>
       </c>
       <c r="E8">
         <v>186.55603236551863</v>
@@ -3606,28 +3522,19 @@
       <c r="AF8">
         <v>186.55603236551863</v>
       </c>
-      <c r="AG8">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AH8">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AI8">
-        <v>186.55603236551863</v>
-      </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>2025</v>
+        <v>285</v>
       </c>
       <c r="C9">
-        <v>2030</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
+        <v>285</v>
+      </c>
+      <c r="D9">
+        <v>285</v>
       </c>
       <c r="E9">
         <v>285</v>
@@ -3713,28 +3620,19 @@
       <c r="AF9">
         <v>285</v>
       </c>
-      <c r="AG9">
-        <v>285</v>
-      </c>
-      <c r="AH9">
-        <v>285</v>
-      </c>
-      <c r="AI9">
-        <v>285</v>
-      </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>2020</v>
+        <v>285</v>
       </c>
       <c r="C10">
-        <v>2030</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
+        <v>285</v>
+      </c>
+      <c r="D10">
+        <v>285</v>
       </c>
       <c r="E10">
         <v>285</v>
@@ -3820,28 +3718,19 @@
       <c r="AF10">
         <v>285</v>
       </c>
-      <c r="AG10">
-        <v>285</v>
-      </c>
-      <c r="AH10">
-        <v>285</v>
-      </c>
-      <c r="AI10">
-        <v>285</v>
-      </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>2028</v>
+        <v>328.60919463891491</v>
       </c>
       <c r="C11">
-        <v>2070</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
+        <v>328.60919463891491</v>
+      </c>
+      <c r="D11">
+        <v>328.60919463891491</v>
       </c>
       <c r="E11">
         <v>328.60919463891491</v>
@@ -3868,194 +3757,176 @@
         <v>328.60919463891491</v>
       </c>
       <c r="M11">
-        <v>328.60919463891491</v>
+        <v>328.04278649674421</v>
       </c>
       <c r="N11">
-        <v>328.60919463891491</v>
+        <v>327.47735464552562</v>
       </c>
       <c r="O11">
-        <v>328.60919463891491</v>
+        <v>326.91289740247259</v>
       </c>
       <c r="P11">
-        <v>328.04278649674421</v>
+        <v>326.34941308769908</v>
       </c>
       <c r="Q11">
-        <v>327.47735464552562</v>
+        <v>325.78690002421456</v>
       </c>
       <c r="R11">
-        <v>326.91289740247259</v>
+        <v>325.22535653791914</v>
       </c>
       <c r="S11">
-        <v>326.34941308769908</v>
+        <v>324.6647809575984</v>
       </c>
       <c r="T11">
-        <v>325.78690002421456</v>
+        <v>324.1051716149185</v>
       </c>
       <c r="U11">
-        <v>325.22535653791914</v>
+        <v>323.54652684442129</v>
       </c>
       <c r="V11">
-        <v>324.6647809575984</v>
+        <v>322.9888449835193</v>
       </c>
       <c r="W11">
-        <v>324.1051716149185</v>
+        <v>322.43212437249076</v>
       </c>
       <c r="X11">
-        <v>323.54652684442129</v>
+        <v>321.87636335447462</v>
       </c>
       <c r="Y11">
-        <v>322.9888449835193</v>
+        <v>321.3215602754658</v>
       </c>
       <c r="Z11">
-        <v>322.43212437249076</v>
+        <v>320.76771348431009</v>
       </c>
       <c r="AA11">
-        <v>321.87636335447462</v>
+        <v>320.21482133269933</v>
       </c>
       <c r="AB11">
-        <v>321.3215602754658</v>
+        <v>319.66288217516637</v>
       </c>
       <c r="AC11">
-        <v>320.76771348431009</v>
+        <v>319.1118943690804</v>
       </c>
       <c r="AD11">
-        <v>320.21482133269933</v>
+        <v>318.56185627464185</v>
       </c>
       <c r="AE11">
-        <v>319.66288217516637</v>
+        <v>318.01276625487765</v>
       </c>
       <c r="AF11">
-        <v>319.1118943690804</v>
-      </c>
-      <c r="AG11">
-        <v>318.56185627464185</v>
-      </c>
-      <c r="AH11">
-        <v>318.01276625487765</v>
-      </c>
-      <c r="AI11">
         <v>317.46462267563663</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>2028</v>
+        <v>172.60979451817616</v>
       </c>
       <c r="C12">
-        <v>2070</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
+        <v>166.55587701007056</v>
+      </c>
+      <c r="D12">
+        <v>160.71428764532004</v>
       </c>
       <c r="E12">
-        <v>172.60979451817616</v>
+        <v>155.07757947070792</v>
       </c>
       <c r="F12">
-        <v>166.55587701007056</v>
+        <v>149.63856671889388</v>
       </c>
       <c r="G12">
-        <v>160.71428764532004</v>
+        <v>144.39031564788095</v>
       </c>
       <c r="H12">
-        <v>155.07757947070792</v>
+        <v>139.32613570176812</v>
       </c>
       <c r="I12">
-        <v>149.63856671889388</v>
+        <v>134.43957098152094</v>
       </c>
       <c r="J12">
-        <v>144.39031564788095</v>
+        <v>129.72439201488626</v>
       </c>
       <c r="K12">
-        <v>139.32613570176812</v>
+        <v>125.17458781495961</v>
       </c>
       <c r="L12">
-        <v>134.43957098152094</v>
+        <v>120.78435821728127</v>
       </c>
       <c r="M12">
-        <v>129.72439201488626</v>
+        <v>120.11336800164422</v>
       </c>
       <c r="N12">
-        <v>125.17458781495961</v>
+        <v>119.44610532056649</v>
       </c>
       <c r="O12">
-        <v>120.78435821728127</v>
+        <v>118.78254946657194</v>
       </c>
       <c r="P12">
-        <v>120.11336800164422</v>
+        <v>118.1226798472201</v>
       </c>
       <c r="Q12">
-        <v>119.44610532056649</v>
+        <v>117.46647598446718</v>
       </c>
       <c r="R12">
-        <v>118.78254946657194</v>
+        <v>116.81391751403054</v>
       </c>
       <c r="S12">
-        <v>118.1226798472201</v>
+        <v>116.16498418475668</v>
       </c>
       <c r="T12">
-        <v>117.46647598446718</v>
+        <v>115.51965585799282</v>
       </c>
       <c r="U12">
-        <v>116.81391751403054</v>
+        <v>114.87791250696193</v>
       </c>
       <c r="V12">
-        <v>116.16498418475668</v>
+        <v>114.23973421614123</v>
       </c>
       <c r="W12">
-        <v>115.51965585799282</v>
+        <v>113.60510118064408</v>
       </c>
       <c r="X12">
-        <v>114.87791250696193</v>
+        <v>112.97399370560547</v>
       </c>
       <c r="Y12">
-        <v>114.23973421614123</v>
+        <v>112.34639220557069</v>
       </c>
       <c r="Z12">
-        <v>113.60510118064408</v>
+        <v>111.72227720388769</v>
       </c>
       <c r="AA12">
-        <v>112.97399370560547</v>
+        <v>111.10162933210248</v>
       </c>
       <c r="AB12">
-        <v>112.34639220557069</v>
+        <v>110.48442932935818</v>
       </c>
       <c r="AC12">
-        <v>111.72227720388769</v>
+        <v>109.87065804179724</v>
       </c>
       <c r="AD12">
-        <v>111.10162933210248</v>
+        <v>109.26029642196706</v>
       </c>
       <c r="AE12">
-        <v>110.48442932935818</v>
+        <v>108.65332552822881</v>
       </c>
       <c r="AF12">
-        <v>109.87065804179724</v>
-      </c>
-      <c r="AG12">
-        <v>109.26029642196706</v>
-      </c>
-      <c r="AH12">
-        <v>108.65332552822881</v>
-      </c>
-      <c r="AI12">
         <v>108.0497265241696</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>2051</v>
+        <v>44.318514766423839</v>
       </c>
       <c r="C13">
-        <v>2070</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
+        <v>44.318514766423839</v>
+      </c>
+      <c r="D13">
+        <v>44.318514766423839</v>
       </c>
       <c r="E13">
         <v>44.318514766423839</v>
@@ -4141,242 +4012,215 @@
       <c r="AF13">
         <v>44.318514766423839</v>
       </c>
-      <c r="AG13">
-        <v>44.318514766423839</v>
-      </c>
-      <c r="AH13">
-        <v>44.318514766423839</v>
-      </c>
-      <c r="AI13">
-        <v>44.318514766423839</v>
-      </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>2035</v>
+        <v>189.63568281915599</v>
       </c>
       <c r="C14">
-        <v>2070</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
+        <v>189.26974337647857</v>
+      </c>
+      <c r="D14">
+        <v>188.90451008611234</v>
       </c>
       <c r="E14">
-        <v>189.63568281915599</v>
+        <v>188.53998158539719</v>
       </c>
       <c r="F14">
-        <v>189.26974337647857</v>
+        <v>188.17615651430248</v>
       </c>
       <c r="G14">
-        <v>188.90451008611234</v>
+        <v>187.81303351542209</v>
       </c>
       <c r="H14">
-        <v>188.53998158539719</v>
+        <v>187.45061123396923</v>
       </c>
       <c r="I14">
-        <v>188.17615651430248</v>
+        <v>187.08888831777145</v>
       </c>
       <c r="J14">
-        <v>187.81303351542209</v>
+        <v>186.72786341726561</v>
       </c>
       <c r="K14">
-        <v>187.45061123396923</v>
+        <v>186.36753518549278</v>
       </c>
       <c r="L14">
-        <v>187.08888831777145</v>
+        <v>186.00790227809333</v>
       </c>
       <c r="M14">
-        <v>186.72786341726561</v>
+        <v>185.54358186639232</v>
       </c>
       <c r="N14">
-        <v>186.36753518549278</v>
+        <v>185.08042050998992</v>
       </c>
       <c r="O14">
-        <v>186.00790227809333</v>
+        <v>184.61841531560569</v>
       </c>
       <c r="P14">
-        <v>185.54358186639232</v>
+        <v>184.15756339718143</v>
       </c>
       <c r="Q14">
-        <v>185.08042050998992</v>
+        <v>183.69786187586331</v>
       </c>
       <c r="R14">
-        <v>184.61841531560569</v>
+        <v>183.23930787998376</v>
       </c>
       <c r="S14">
-        <v>184.15756339718143</v>
+        <v>182.78189854504356</v>
       </c>
       <c r="T14">
-        <v>183.69786187586331</v>
+        <v>182.32563101369405</v>
       </c>
       <c r="U14">
-        <v>183.23930787998376</v>
+        <v>181.87050243571915</v>
       </c>
       <c r="V14">
-        <v>182.78189854504356</v>
+        <v>181.41650996801758</v>
       </c>
       <c r="W14">
-        <v>182.32563101369405</v>
+        <v>180.96365077458518</v>
       </c>
       <c r="X14">
-        <v>181.87050243571915</v>
+        <v>180.5119220264971</v>
       </c>
       <c r="Y14">
-        <v>181.41650996801758</v>
+        <v>180.06132090189018</v>
       </c>
       <c r="Z14">
-        <v>180.96365077458518</v>
+        <v>179.61184458594531</v>
       </c>
       <c r="AA14">
-        <v>180.5119220264971</v>
+        <v>179.1634902708698</v>
       </c>
       <c r="AB14">
-        <v>180.06132090189018</v>
+        <v>178.71625515587996</v>
       </c>
       <c r="AC14">
-        <v>179.61184458594531</v>
+        <v>178.27013644718349</v>
       </c>
       <c r="AD14">
-        <v>179.1634902708698</v>
+        <v>177.82513135796208</v>
       </c>
       <c r="AE14">
-        <v>178.71625515587996</v>
+        <v>177.38123710835396</v>
       </c>
       <c r="AF14">
-        <v>178.27013644718349</v>
-      </c>
-      <c r="AG14">
-        <v>177.82513135796208</v>
-      </c>
-      <c r="AH14">
-        <v>177.38123710835396</v>
-      </c>
-      <c r="AI14">
         <v>176.93845092543677</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>2025</v>
+        <v>225.22825093854229</v>
       </c>
       <c r="C15">
-        <v>2070</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
+        <v>224.72915840008622</v>
+      </c>
+      <c r="D15">
+        <v>224.23117182129951</v>
       </c>
       <c r="E15">
-        <v>225.22825093854229</v>
+        <v>223.73428875144072</v>
       </c>
       <c r="F15">
-        <v>224.72915840008622</v>
+        <v>223.238506745199</v>
       </c>
       <c r="G15">
-        <v>224.23117182129951</v>
+        <v>222.74382336268226</v>
       </c>
       <c r="H15">
-        <v>223.73428875144072</v>
+        <v>222.25023616940504</v>
       </c>
       <c r="I15">
-        <v>223.238506745199</v>
+        <v>221.75774273627653</v>
       </c>
       <c r="J15">
-        <v>222.74382336268226</v>
+        <v>221.26634063958866</v>
       </c>
       <c r="K15">
-        <v>222.25023616940504</v>
+        <v>220.77602746100419</v>
       </c>
       <c r="L15">
-        <v>221.75774273627653</v>
+        <v>220.28680078754479</v>
       </c>
       <c r="M15">
-        <v>221.26634063958866</v>
+        <v>219.27722536643881</v>
       </c>
       <c r="N15">
-        <v>220.77602746100419</v>
+        <v>218.27227683413079</v>
       </c>
       <c r="O15">
-        <v>220.28680078754479</v>
+        <v>217.27193398556807</v>
       </c>
       <c r="P15">
-        <v>219.27722536643881</v>
+        <v>216.2761757128809</v>
       </c>
       <c r="Q15">
-        <v>218.27227683413079</v>
+        <v>215.28498100493692</v>
       </c>
       <c r="R15">
-        <v>217.27193398556807</v>
+        <v>214.29832894689795</v>
       </c>
       <c r="S15">
-        <v>216.2761757128809</v>
+        <v>213.31619871977858</v>
       </c>
       <c r="T15">
-        <v>215.28498100493692</v>
+        <v>212.33856960000691</v>
       </c>
       <c r="U15">
-        <v>214.29832894689795</v>
+        <v>211.36542095898724</v>
       </c>
       <c r="V15">
-        <v>213.31619871977858</v>
+        <v>210.39673226266487</v>
       </c>
       <c r="W15">
-        <v>212.33856960000691</v>
+        <v>209.43248307109272</v>
       </c>
       <c r="X15">
-        <v>211.36542095898724</v>
+        <v>208.47265303800012</v>
       </c>
       <c r="Y15">
-        <v>210.39673226266487</v>
+        <v>207.51722191036345</v>
       </c>
       <c r="Z15">
-        <v>209.43248307109272</v>
+        <v>206.56616952797873</v>
       </c>
       <c r="AA15">
-        <v>208.47265303800012</v>
+        <v>205.61947582303637</v>
       </c>
       <c r="AB15">
-        <v>207.51722191036345</v>
+        <v>204.67712081969759</v>
       </c>
       <c r="AC15">
-        <v>206.56616952797873</v>
+        <v>203.739084633673</v>
       </c>
       <c r="AD15">
-        <v>205.61947582303637</v>
+        <v>202.80534747180297</v>
       </c>
       <c r="AE15">
-        <v>204.67712081969759</v>
+        <v>201.87588963164006</v>
       </c>
       <c r="AF15">
-        <v>203.739084633673</v>
-      </c>
-      <c r="AG15">
-        <v>202.80534747180297</v>
-      </c>
-      <c r="AH15">
-        <v>201.87588963164006</v>
-      </c>
-      <c r="AI15">
         <v>200.95069150103299</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>2028</v>
+        <v>186.55603236551863</v>
       </c>
       <c r="C16">
-        <v>2070</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
+        <v>186.55603236551863</v>
+      </c>
+      <c r="D16">
+        <v>186.55603236551863</v>
       </c>
       <c r="E16">
         <v>186.55603236551863</v>
@@ -4462,28 +4306,19 @@
       <c r="AF16">
         <v>186.55603236551863</v>
       </c>
-      <c r="AG16">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AH16">
-        <v>186.55603236551863</v>
-      </c>
-      <c r="AI16">
-        <v>186.55603236551863</v>
-      </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>2020</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>2070</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4569,28 +4404,19 @@
       <c r="AF17">
         <v>0</v>
       </c>
-      <c r="AG17">
-        <v>0</v>
-      </c>
-      <c r="AH17">
-        <v>0</v>
-      </c>
-      <c r="AI17">
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>2020</v>
+        <v>125.411</v>
       </c>
       <c r="C18">
-        <v>2070</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
+        <v>125.411</v>
+      </c>
+      <c r="D18">
+        <v>125.411</v>
       </c>
       <c r="E18">
         <v>125.411</v>
@@ -4676,28 +4502,19 @@
       <c r="AF18">
         <v>125.411</v>
       </c>
-      <c r="AG18">
-        <v>125.411</v>
-      </c>
-      <c r="AH18">
-        <v>125.411</v>
-      </c>
-      <c r="AI18">
-        <v>125.411</v>
-      </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>2028</v>
+        <v>346.89636968559745</v>
       </c>
       <c r="C19">
-        <v>2070</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
+        <v>346.89636968559745</v>
+      </c>
+      <c r="D19">
+        <v>346.89636968559745</v>
       </c>
       <c r="E19">
         <v>346.89636968559745</v>
@@ -4724,87 +4541,78 @@
         <v>346.89636968559745</v>
       </c>
       <c r="M19">
-        <v>346.89636968559745</v>
+        <v>346.08781589360348</v>
       </c>
       <c r="N19">
-        <v>346.89636968559745</v>
+        <v>345.28114669681338</v>
       </c>
       <c r="O19">
-        <v>346.89636968559745</v>
+        <v>344.47635770257062</v>
       </c>
       <c r="P19">
-        <v>346.08781589360348</v>
+        <v>343.67344452845725</v>
       </c>
       <c r="Q19">
-        <v>345.28114669681338</v>
+        <v>342.87240280226985</v>
       </c>
       <c r="R19">
-        <v>344.47635770257062</v>
+        <v>342.07322816199581</v>
       </c>
       <c r="S19">
-        <v>343.67344452845725</v>
+        <v>341.27591625578975</v>
       </c>
       <c r="T19">
-        <v>342.87240280226985</v>
+        <v>340.48046274194951</v>
       </c>
       <c r="U19">
-        <v>342.07322816199581</v>
+        <v>339.68686328889277</v>
       </c>
       <c r="V19">
-        <v>341.27591625578975</v>
+        <v>338.89511357513334</v>
       </c>
       <c r="W19">
-        <v>340.48046274194951</v>
+        <v>338.10520928925757</v>
       </c>
       <c r="X19">
-        <v>339.68686328889277</v>
+        <v>337.31714612990106</v>
       </c>
       <c r="Y19">
-        <v>338.89511357513334</v>
+        <v>336.53091980572503</v>
       </c>
       <c r="Z19">
-        <v>338.10520928925757</v>
+        <v>335.74652603539317</v>
       </c>
       <c r="AA19">
-        <v>337.31714612990106</v>
+        <v>334.96396054754803</v>
       </c>
       <c r="AB19">
-        <v>336.53091980572503</v>
+        <v>334.18321908078809</v>
       </c>
       <c r="AC19">
-        <v>335.74652603539317</v>
+        <v>333.40429738364435</v>
       </c>
       <c r="AD19">
-        <v>334.96396054754803</v>
+        <v>332.62719121455717</v>
       </c>
       <c r="AE19">
-        <v>334.18321908078809</v>
+        <v>331.85189634185332</v>
       </c>
       <c r="AF19">
-        <v>333.40429738364435</v>
-      </c>
-      <c r="AG19">
-        <v>332.62719121455717</v>
-      </c>
-      <c r="AH19">
-        <v>331.85189634185332</v>
-      </c>
-      <c r="AI19">
         <v>331.07840854372256</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>2028</v>
+        <v>178.07271343191354</v>
       </c>
       <c r="C20">
-        <v>2070</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
+        <v>178.07271343191354</v>
+      </c>
+      <c r="D20">
+        <v>178.07271343191354</v>
       </c>
       <c r="E20">
         <v>178.07271343191354</v>
@@ -4831,87 +4639,78 @@
         <v>178.07271343191354</v>
       </c>
       <c r="M20">
-        <v>178.07271343191354</v>
+        <v>177.85430515702365</v>
       </c>
       <c r="N20">
-        <v>178.07271343191354</v>
+        <v>177.6361647624486</v>
       </c>
       <c r="O20">
-        <v>178.07271343191354</v>
+        <v>177.41829191963006</v>
       </c>
       <c r="P20">
-        <v>177.85430515702365</v>
+        <v>177.20068630041266</v>
       </c>
       <c r="Q20">
-        <v>177.6361647624486</v>
+        <v>176.98334757704347</v>
       </c>
       <c r="R20">
-        <v>177.41829191963006</v>
+        <v>176.76627542217165</v>
       </c>
       <c r="S20">
-        <v>177.20068630041266</v>
+        <v>176.54946950884778</v>
       </c>
       <c r="T20">
-        <v>176.98334757704347</v>
+        <v>176.33292951052346</v>
       </c>
       <c r="U20">
-        <v>176.76627542217165</v>
+        <v>176.11665510105084</v>
       </c>
       <c r="V20">
-        <v>176.54946950884778</v>
+        <v>175.90064595468206</v>
       </c>
       <c r="W20">
-        <v>176.33292951052346</v>
+        <v>175.68490174606882</v>
       </c>
       <c r="X20">
-        <v>176.11665510105084</v>
+        <v>175.46942215026186</v>
       </c>
       <c r="Y20">
-        <v>175.90064595468206</v>
+        <v>175.25420684271046</v>
       </c>
       <c r="Z20">
-        <v>175.68490174606882</v>
+        <v>175.03925549926194</v>
       </c>
       <c r="AA20">
-        <v>175.46942215026186</v>
+        <v>174.82456779616126</v>
       </c>
       <c r="AB20">
-        <v>175.25420684271046</v>
+        <v>174.61014341005043</v>
       </c>
       <c r="AC20">
-        <v>175.03925549926194</v>
+        <v>174.39598201796804</v>
       </c>
       <c r="AD20">
-        <v>174.82456779616126</v>
+        <v>174.18208329734887</v>
       </c>
       <c r="AE20">
-        <v>174.61014341005043</v>
+        <v>173.96844692602326</v>
       </c>
       <c r="AF20">
-        <v>174.39598201796804</v>
-      </c>
-      <c r="AG20">
-        <v>174.18208329734887</v>
-      </c>
-      <c r="AH20">
-        <v>173.96844692602326</v>
-      </c>
-      <c r="AI20">
         <v>173.75507258221657</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>2028</v>
+        <v>161.17759706353402</v>
       </c>
       <c r="C21">
-        <v>2070</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
+        <v>161.17759706353402</v>
+      </c>
+      <c r="D21">
+        <v>161.17759706353402</v>
       </c>
       <c r="E21">
         <v>161.17759706353402</v>
@@ -4997,135 +4796,117 @@
       <c r="AF21">
         <v>161.17759706353402</v>
       </c>
-      <c r="AG21">
-        <v>161.17759706353402</v>
-      </c>
-      <c r="AH21">
-        <v>161.17759706353402</v>
-      </c>
-      <c r="AI21">
-        <v>161.17759706353402</v>
-      </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>2035</v>
+        <v>198.91350448271311</v>
       </c>
       <c r="C22">
-        <v>2070</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
+        <v>198.36169823946378</v>
+      </c>
+      <c r="D22">
+        <v>197.81142276271962</v>
       </c>
       <c r="E22">
-        <v>198.91350448271311</v>
+        <v>197.26267380597903</v>
       </c>
       <c r="F22">
-        <v>198.36169823946378</v>
+        <v>196.71544713452064</v>
       </c>
       <c r="G22">
-        <v>197.81142276271962</v>
+        <v>196.16973852537063</v>
       </c>
       <c r="H22">
-        <v>197.26267380597903</v>
+        <v>195.62554376727013</v>
       </c>
       <c r="I22">
-        <v>196.71544713452064</v>
+        <v>195.08285866064276</v>
       </c>
       <c r="J22">
-        <v>196.16973852537063</v>
+        <v>194.54167901756213</v>
       </c>
       <c r="K22">
-        <v>195.62554376727013</v>
+        <v>194.00200066171962</v>
       </c>
       <c r="L22">
-        <v>195.08285866064276</v>
+        <v>193.46381942839218</v>
       </c>
       <c r="M22">
-        <v>194.54167901756213</v>
+        <v>192.4623741389203</v>
       </c>
       <c r="N22">
-        <v>194.00200066171962</v>
+        <v>191.46611272657213</v>
       </c>
       <c r="O22">
-        <v>193.46381942839218</v>
+        <v>190.47500835754829</v>
       </c>
       <c r="P22">
-        <v>192.4623741389203</v>
+        <v>189.4890343369517</v>
       </c>
       <c r="Q22">
-        <v>191.46611272657213</v>
+        <v>188.50816410806866</v>
       </c>
       <c r="R22">
-        <v>190.47500835754829</v>
+        <v>187.5323712516535</v>
       </c>
       <c r="S22">
-        <v>189.4890343369517</v>
+        <v>186.56162948521705</v>
       </c>
       <c r="T22">
-        <v>188.50816410806866</v>
+        <v>185.59591266231868</v>
       </c>
       <c r="U22">
-        <v>187.5323712516535</v>
+        <v>184.63519477186213</v>
       </c>
       <c r="V22">
-        <v>186.56162948521705</v>
+        <v>183.67944993739479</v>
       </c>
       <c r="W22">
-        <v>185.59591266231868</v>
+        <v>182.72865241641091</v>
       </c>
       <c r="X22">
-        <v>184.63519477186213</v>
+        <v>181.78277659965804</v>
       </c>
       <c r="Y22">
-        <v>183.67944993739479</v>
+        <v>180.84179701044741</v>
       </c>
       <c r="Z22">
-        <v>182.72865241641091</v>
+        <v>179.90568830396765</v>
       </c>
       <c r="AA22">
-        <v>181.78277659965804</v>
+        <v>178.9744252666022</v>
       </c>
       <c r="AB22">
-        <v>180.84179701044741</v>
+        <v>178.04798281525012</v>
       </c>
       <c r="AC22">
-        <v>179.90568830396765</v>
+        <v>177.12633599665054</v>
       </c>
       <c r="AD22">
-        <v>178.9744252666022</v>
+        <v>176.20945998671053</v>
       </c>
       <c r="AE22">
-        <v>178.04798281525012</v>
+        <v>175.29733008983649</v>
       </c>
       <c r="AF22">
-        <v>177.12633599665054</v>
-      </c>
-      <c r="AG22">
-        <v>176.20945998671053</v>
-      </c>
-      <c r="AH22">
-        <v>175.29733008983649</v>
-      </c>
-      <c r="AI22">
         <v>174.38992173826901</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>2028</v>
+        <v>341.77033776951453</v>
       </c>
       <c r="C23">
-        <v>2070</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
+        <v>341.77033776951453</v>
+      </c>
+      <c r="D23">
+        <v>341.77033776951453</v>
       </c>
       <c r="E23">
         <v>341.77033776951453</v>
@@ -5152,72 +4933,63 @@
         <v>341.77033776951453</v>
       </c>
       <c r="M23">
-        <v>341.77033776951453</v>
+        <v>341.02989577410909</v>
       </c>
       <c r="N23">
-        <v>341.77033776951453</v>
+        <v>340.29105793883099</v>
       </c>
       <c r="O23">
-        <v>341.77033776951453</v>
+        <v>339.55382078828347</v>
       </c>
       <c r="P23">
-        <v>341.02989577410909</v>
+        <v>338.81818085459918</v>
       </c>
       <c r="Q23">
-        <v>340.29105793883099</v>
+        <v>338.08413467742389</v>
       </c>
       <c r="R23">
-        <v>339.55382078828347</v>
+        <v>337.35167880390014</v>
       </c>
       <c r="S23">
-        <v>338.81818085459918</v>
+        <v>336.62080978865112</v>
       </c>
       <c r="T23">
-        <v>338.08413467742389</v>
+        <v>335.89152419376433</v>
       </c>
       <c r="U23">
-        <v>337.35167880390014</v>
+        <v>335.16381858877548</v>
       </c>
       <c r="V23">
-        <v>336.62080978865112</v>
+        <v>334.43768955065241</v>
       </c>
       <c r="W23">
-        <v>335.89152419376433</v>
+        <v>333.71313366377882</v>
       </c>
       <c r="X23">
-        <v>335.16381858877548</v>
+        <v>332.99014751993843</v>
       </c>
       <c r="Y23">
-        <v>334.43768955065241</v>
+        <v>332.26872771829875</v>
       </c>
       <c r="Z23">
-        <v>333.71313366377882</v>
+        <v>331.54887086539514</v>
       </c>
       <c r="AA23">
-        <v>332.99014751993843</v>
+        <v>330.8305735751149</v>
       </c>
       <c r="AB23">
-        <v>332.26872771829875</v>
+        <v>330.11383246868132</v>
       </c>
       <c r="AC23">
-        <v>331.54887086539514</v>
+        <v>329.39864417463781</v>
       </c>
       <c r="AD23">
-        <v>330.8305735751149</v>
+        <v>328.68500532883195</v>
       </c>
       <c r="AE23">
-        <v>330.11383246868132</v>
+        <v>327.97291257439969</v>
       </c>
       <c r="AF23">
-        <v>329.39864417463781</v>
-      </c>
-      <c r="AG23">
-        <v>328.68500532883195</v>
-      </c>
-      <c r="AH23">
-        <v>327.97291257439969</v>
-      </c>
-      <c r="AI23">
         <v>327.26236256174968</v>
       </c>
     </row>
@@ -5230,18 +5002,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DCA1AF-7FFF-485C-ACA8-5A2E538B55BD}">
   <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -5337,9 +5109,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>123.67359046905142</v>
@@ -5435,9 +5207,9 @@
         <v>123.67359046905142</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>129.7454074415285</v>
@@ -5533,9 +5305,9 @@
         <v>129.7454074415285</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>118.2709560009595</v>
@@ -5631,9 +5403,9 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>115.19221945755521</v>
@@ -5729,9 +5501,9 @@
         <v>107.6672142896653</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>115.31289132206044</v>
@@ -5827,9 +5599,9 @@
         <v>115.31289132206044</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>118.2709560009595</v>
@@ -5925,9 +5697,9 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>118.2709560009595</v>
@@ -6023,9 +5795,9 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>129.7454074415285</v>
@@ -6121,9 +5893,9 @@
         <v>129.7454074415285</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>129.7454074415285</v>
@@ -6219,9 +5991,9 @@
         <v>129.7454074415285</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>183.80157163059505</v>
@@ -6317,9 +6089,9 @@
         <v>182.50258040856943</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>116.64540765296805</v>
@@ -6415,9 +6187,9 @@
         <v>109.12040248507815</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>123.67359046905142</v>
@@ -6513,9 +6285,9 @@
         <v>123.67359046905142</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>118.62991450733945</v>
@@ -6611,9 +6383,9 @@
         <v>117.14994804220183</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>144.49298389836392</v>
@@ -6709,9 +6481,9 @@
         <v>141.66323532610448</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>118.2709560009595</v>
@@ -6807,9 +6579,9 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>526.20000000000005</v>
@@ -6905,9 +6677,9 @@
         <v>526.20000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>62.986140000000006</v>
@@ -7003,9 +6775,9 @@
         <v>62.986140000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>139.03817460704778</v>
@@ -7101,9 +6873,9 @@
         <v>137.19446156527806</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>136.25538273848147</v>
@@ -7199,9 +6971,9 @@
         <v>135.75212630278384</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>115.31289132206044</v>
@@ -7297,9 +7069,9 @@
         <v>115.31289132206044</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>119.71132067889909</v>
@@ -7395,9 +7167,9 @@
         <v>116.8528960733945</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>200.11558338601148</v>
@@ -7499,8 +7271,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="319a675c9647c7594acaff66597be50a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88dc2720d39439db86350823647c6b2d" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -7519,6 +7291,8 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7571,6 +7345,16 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -7721,13 +7505,48 @@
         <AccountId>30706</AccountId>
         <AccountType/>
       </UserInfo>
+      <UserInfo>
+        <DisplayName>Hugo Stevens</DisplayName>
+        <AccountId>35233</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Aparajit Pandey</DisplayName>
+        <AccountId>16740</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Natera</DisplayName>
+        <AccountId>34591</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jason Martins</DisplayName>
+        <AccountId>29512</AccountId>
+        <AccountType/>
+      </UserInfo>
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{621E4A8A-3A20-4BCE-A4A6-D2B9AEED33CE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF42D93C-9214-42FE-B104-7B90E676C82E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
+    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>